<commit_message>
eliminiting old tables to the puclication
</commit_message>
<xml_diff>
--- a/table 1.xlsx
+++ b/table 1.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/enieto/Library/Mobile Documents/com~apple~CloudDocs/Documents/Documents - pe-dmue-mbp22/Subtratum_evaluation_foliar_soybean/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F7351BB-43CA-4640-9E1C-4745DE1CF8CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF4E10D2-E48F-2E45-9477-626BED85FB04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="580" windowWidth="13000" windowHeight="16380" activeTab="1" xr2:uid="{49DC0FC8-E60A-2C47-9FE5-591EB2DDFB5C}"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="26240" windowHeight="15240" activeTab="3" xr2:uid="{49DC0FC8-E60A-2C47-9FE5-591EB2DDFB5C}"/>
   </bookViews>
   <sheets>
     <sheet name="table1" sheetId="1" r:id="rId1"/>
     <sheet name="table1 (2)" sheetId="3" r:id="rId2"/>
     <sheet name="table2" sheetId="2" r:id="rId3"/>
+    <sheet name="Supplemental data" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="103">
   <si>
     <t>condition  </t>
   </si>
@@ -308,13 +309,52 @@
   </si>
   <si>
     <t>groups</t>
+  </si>
+  <si>
+    <t>asymp.LCL</t>
+  </si>
+  <si>
+    <t>asymp.UCL</t>
+  </si>
+  <si>
+    <t>Ingredients per L</t>
+  </si>
+  <si>
+    <t>35 g GerberⓇ 1st foodsⓇ green bean baby food + 20 g BD DifcoTM Agar</t>
+  </si>
+  <si>
+    <t>Soybean Stem Broth</t>
+  </si>
+  <si>
+    <t>Lima Bean Broth</t>
+  </si>
+  <si>
+    <t>Broths</t>
+  </si>
+  <si>
+    <t>960 mL DI, 40 mL V8 juice strained through a metal strainer,  0.6 g Calcium Carbonate, 0.2 g BD Bacto yeast extract, 1 g Sucrose, 20 g  BD DifcoTM Agar</t>
+  </si>
+  <si>
+    <t>500 mL Soybean Stem Broth, 250 mL Lima Bean Broth,  250 mL of DI water</t>
+  </si>
+  <si>
+    <t>100 g Soybean-stems cuts,1100mL DI water and autoclave at 121°C for 60 minutes</t>
+  </si>
+  <si>
+    <t>400 g Lima beans, 1300mL DI water and autoclave at 121°C for 60 minutes</t>
+  </si>
+  <si>
+    <t>For both broths filter out each  using 4 layers of cheesecloth and, If volume is below 1000mL, adjust to 1000mL with DI water, save in the freezer In need the leaftovers fro later use</t>
+  </si>
+  <si>
+    <t>39 g of PDA BD DifcoTM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -326,6 +366,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -384,7 +430,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -400,7 +446,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -416,6 +461,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1070,8 +1130,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06C86B41-A5E8-9345-9AAD-A6481BC5A675}">
   <dimension ref="A1:P19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1169,16 +1229,16 @@
       <c r="A5" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="B5" s="15">
+      <c r="B5" s="14">
         <v>17.399999999999999</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="14">
         <v>15.56</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="14">
         <v>44</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="14">
         <v>2.35</v>
       </c>
       <c r="F5" s="8">
@@ -1192,16 +1252,16 @@
       <c r="A6" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="B6" s="15">
+      <c r="B6" s="14">
         <v>13.02</v>
       </c>
-      <c r="C6" s="15">
+      <c r="C6" s="14">
         <v>20.87</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="14">
         <v>38</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E6" s="14">
         <v>3.39</v>
       </c>
       <c r="F6" s="8">
@@ -1215,16 +1275,16 @@
       <c r="A7" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B7" s="15">
+      <c r="B7" s="14">
         <v>11.11</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="14">
         <v>11.04</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="14">
         <v>44</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="14">
         <v>1.66</v>
       </c>
       <c r="F7" s="8">
@@ -1238,16 +1298,16 @@
       <c r="A8" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B8" s="15">
+      <c r="B8" s="14">
         <v>7.32</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C8" s="14">
         <v>10.37</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="14">
         <v>43</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E8" s="14">
         <v>1.58</v>
       </c>
       <c r="F8" s="8">
@@ -1261,16 +1321,16 @@
       <c r="A9" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B9" s="15">
+      <c r="B9" s="14">
         <v>4.09</v>
       </c>
-      <c r="C9" s="15">
+      <c r="C9" s="14">
         <v>5.13</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="14">
         <v>45</v>
       </c>
-      <c r="E9" s="15">
+      <c r="E9" s="14">
         <v>0.76</v>
       </c>
       <c r="F9" s="8">
@@ -1281,15 +1341,15 @@
       <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A10" s="14"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
+      <c r="A10" s="13"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="K14" s="7"/>
@@ -1349,7 +1409,7 @@
   <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E11"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1360,22 +1420,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="12" t="s">
         <v>74</v>
       </c>
       <c r="E1" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="G1" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="F1" s="9"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
@@ -1390,10 +1455,23 @@
       <c r="D2" s="8">
         <v>5.47</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2">
+        <f>ROUND(J2,2)</f>
+        <v>13.3</v>
+      </c>
+      <c r="F2">
+        <f>ROUND(K2,2)</f>
+        <v>45.95</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="F2" s="1"/>
+      <c r="J2" s="8">
+        <v>13.302490000000001</v>
+      </c>
+      <c r="K2" s="8">
+        <v>45.945404000000003</v>
+      </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
@@ -1408,10 +1486,23 @@
       <c r="D3" s="8">
         <v>4.8600000000000003</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3">
+        <f t="shared" ref="E3:E11" si="0">ROUND(J3,2)</f>
+        <v>13.86</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F11" si="1">ROUND(K3,2)</f>
+        <v>42.54</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="F3" s="1"/>
+      <c r="J3" s="8">
+        <v>13.85716</v>
+      </c>
+      <c r="K3" s="8">
+        <v>42.536937999999999</v>
+      </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
@@ -1426,10 +1517,23 @@
       <c r="D4" s="8">
         <v>3.43</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>9.6300000000000008</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>29.86</v>
+      </c>
+      <c r="G4" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="F4" s="1"/>
+      <c r="J4" s="8">
+        <v>9.6342040000000004</v>
+      </c>
+      <c r="K4" s="8">
+        <v>29.857091</v>
+      </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
@@ -1444,10 +1548,23 @@
       <c r="D5" s="8">
         <v>2.4900000000000002</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>6.89</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>21.62</v>
+      </c>
+      <c r="G5" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="F5" s="1"/>
+      <c r="J5" s="8">
+        <v>6.8905779999999996</v>
+      </c>
+      <c r="K5" s="8">
+        <v>21.616607999999999</v>
+      </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
@@ -1462,10 +1579,23 @@
       <c r="D6" s="8">
         <v>2.16</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>5.92</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>18.71</v>
+      </c>
+      <c r="G6" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="F6" s="1"/>
+      <c r="J6" s="8">
+        <v>5.9238580000000001</v>
+      </c>
+      <c r="K6" s="8">
+        <v>18.712026999999999</v>
+      </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
@@ -1480,12 +1610,23 @@
       <c r="D7" s="8">
         <v>1.1200000000000001</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>2.88</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>9.56</v>
+      </c>
+      <c r="G7" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="F7" s="1"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="8"/>
+      <c r="J7" s="8">
+        <v>2.8822920000000001</v>
+      </c>
+      <c r="K7" s="8">
+        <v>9.5627030000000008</v>
+      </c>
       <c r="L7" s="8"/>
       <c r="M7" s="8"/>
       <c r="N7" s="8"/>
@@ -1505,12 +1646,23 @@
       <c r="D8" s="8">
         <v>0.98</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>8.31</v>
+      </c>
+      <c r="G8" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="F8" s="1"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="8"/>
+      <c r="J8" s="8">
+        <v>2.4673189999999998</v>
+      </c>
+      <c r="K8" s="8">
+        <v>8.311242</v>
+      </c>
       <c r="L8" s="8"/>
       <c r="M8" s="8"/>
       <c r="N8" s="8"/>
@@ -1530,12 +1682,23 @@
       <c r="D9" s="8">
         <v>0.8</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>6.75</v>
+      </c>
+      <c r="G9" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="F9" s="1"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="8"/>
+      <c r="J9" s="8">
+        <v>2.0068700000000002</v>
+      </c>
+      <c r="K9" s="8">
+        <v>6.745628</v>
+      </c>
       <c r="L9" s="8"/>
       <c r="M9" s="8"/>
       <c r="N9" s="8"/>
@@ -1555,12 +1718,23 @@
       <c r="D10" s="8">
         <v>0.61</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>1.26</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>4.93</v>
+      </c>
+      <c r="G10" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="F10" s="1"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="8"/>
+      <c r="J10" s="8">
+        <v>1.2605280000000001</v>
+      </c>
+      <c r="K10" s="8">
+        <v>4.933478</v>
+      </c>
       <c r="L10" s="8"/>
       <c r="M10" s="8"/>
       <c r="N10" s="8"/>
@@ -1568,24 +1742,35 @@
       <c r="P10" s="7"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C11" s="10">
         <v>2.21</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D11" s="10">
         <v>0.53</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="4">
+        <f t="shared" si="0"/>
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="F11" s="4">
+        <f t="shared" si="1"/>
+        <v>4.3499999999999996</v>
+      </c>
+      <c r="G11" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="F11" s="9"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="8"/>
+      <c r="J11" s="8">
+        <v>1.1209990000000001</v>
+      </c>
+      <c r="K11" s="8">
+        <v>4.3503480000000003</v>
+      </c>
       <c r="L11" s="8"/>
       <c r="M11" s="8"/>
       <c r="N11" s="8"/>
@@ -1649,4 +1834,86 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24A65DE9-6578-B34E-9EB3-A178D108B76C}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="15.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="170" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="85" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="70" x14ac:dyDescent="0.2">
+      <c r="A4" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="204" x14ac:dyDescent="0.2">
+      <c r="A6" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="98" x14ac:dyDescent="0.2">
+      <c r="A7" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="84" x14ac:dyDescent="0.2">
+      <c r="A8" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>